<commit_message>
added some testcases and pom dependencies
</commit_message>
<xml_diff>
--- a/Automation_Project_7rMart_Supermarket/src/test/resources/TestData.xlsx
+++ b/Automation_Project_7rMart_Supermarket/src/test/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jista\git\Automation_Project_7rMart_Supermarket\Automation_Project_7rMart_Supermarket\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F379D69-EE91-4DDC-B2B0-A2DFAD65BEE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B815282-E9B1-460A-A814-BF95DA7201EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" activeTab="3" xr2:uid="{0C1EF4DA-6666-492B-8CD9-1F9D6C22656A}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>username</t>
   </si>
@@ -90,10 +90,16 @@
     <t>C:\\Users\\TestDocuments\\Sample_img.png</t>
   </si>
   <si>
-    <t>catgeory expected</t>
-  </si>
-  <si>
-    <t>Vehicle</t>
+    <t>categoryStatusExpected</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>category expected</t>
+  </si>
+  <si>
+    <t>Food</t>
   </si>
 </sst>
 </file>
@@ -590,24 +596,31 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3743B6A-AA27-41F9-BD4F-A2336115A58A}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.109375" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
commit after page chaining
</commit_message>
<xml_diff>
--- a/Automation_Project_7rMart_Supermarket/src/test/resources/TestData.xlsx
+++ b/Automation_Project_7rMart_Supermarket/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jista\git\Automation_Project_7rMart_Supermarket\Automation_Project_7rMart_Supermarket\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B815282-E9B1-460A-A814-BF95DA7201EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3AA500B-1F8C-456D-B2D0-2057F00011FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" activeTab="3" xr2:uid="{0C1EF4DA-6666-492B-8CD9-1F9D6C22656A}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" activeTab="2" xr2:uid="{0C1EF4DA-6666-492B-8CD9-1F9D6C22656A}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>username</t>
   </si>
@@ -72,22 +72,10 @@
     <t>staff</t>
   </si>
   <si>
-    <t>imgFilePath</t>
-  </si>
-  <si>
     <t>scrollData</t>
   </si>
   <si>
-    <t>C:\\Users\\TestDocuments\\appliances.jpg</t>
-  </si>
-  <si>
     <t>window.scrollBy(0,450)</t>
-  </si>
-  <si>
-    <t>imgPathLink</t>
-  </si>
-  <si>
-    <t>C:\\Users\\TestDocuments\\Sample_img.png</t>
   </si>
   <si>
     <t>categoryStatusExpected</t>
@@ -554,9 +542,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C54B0B72-AC0A-4FC3-8C43-1F933D96CBFB}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="B1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -567,26 +555,14 @@
     <col min="3" max="3" width="38.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
         <v>15</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -598,7 +574,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3743B6A-AA27-41F9-BD4F-A2336115A58A}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -610,18 +586,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>